<commit_message>
Updated OFS code by considering academic calender
</commit_message>
<xml_diff>
--- a/analysis/data/OFS_CBI.xlsx
+++ b/analysis/data/OFS_CBI.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E89"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,12 +451,17 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>years_offered</t>
+          <t>acad_years_offered</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
           <t>OFS_CBI</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Course Description</t>
         </is>
       </c>
     </row>
@@ -480,6 +485,11 @@
       <c r="E2" t="n">
         <v>3</v>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Applied Cyberinfrastruct Conc</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -501,6 +511,11 @@
       <c r="E3" t="n">
         <v>3</v>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Game AI</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -522,6 +537,11 @@
       <c r="E4" t="n">
         <v>3</v>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Designing an Installation</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -538,10 +558,15 @@
         <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
         <v>3</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Data Ethics</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -559,10 +584,15 @@
         <v>7</v>
       </c>
       <c r="D6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" t="n">
         <v>2</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Foundations of Information</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -580,10 +610,15 @@
         <v>4</v>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Information Research Methods</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -601,10 +636,15 @@
         <v>3</v>
       </c>
       <c r="D8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" t="n">
         <v>3</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Bayesian Modeling &amp; Inference</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -622,10 +662,15 @@
         <v>2</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
         <v>3</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Foundations of Data Science</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -648,6 +693,11 @@
       <c r="E10" t="n">
         <v>3</v>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Computational Social Science</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -664,11 +714,16 @@
         <v>8</v>
       </c>
       <c r="D11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Organization/Information</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -685,11 +740,16 @@
         <v>8</v>
       </c>
       <c r="D12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" t="n">
         <v>1</v>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Intro: Human Computer Interact</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -711,6 +771,11 @@
       <c r="E13" t="n">
         <v>3</v>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Intro to Digital Cultures</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -732,6 +797,11 @@
       <c r="E14" t="n">
         <v>3</v>
       </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Info Trust and Manipulation</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -748,10 +818,15 @@
         <v>7</v>
       </c>
       <c r="D15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E15" t="n">
         <v>2</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Ethical Issues in Information</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -769,11 +844,16 @@
         <v>8</v>
       </c>
       <c r="D16" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E16" t="n">
         <v>1</v>
       </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Intro to Machine Learning</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -790,11 +870,16 @@
         <v>8</v>
       </c>
       <c r="D17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E17" t="n">
         <v>1</v>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Data Mining/Discovery</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -811,11 +896,16 @@
         <v>8</v>
       </c>
       <c r="D18" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E18" t="n">
         <v>1</v>
       </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Virtual Reality</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -835,7 +925,12 @@
         <v>4</v>
       </c>
       <c r="E19" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Algorithms for Games</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -853,11 +948,16 @@
         <v>8</v>
       </c>
       <c r="D20" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
       </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Data Analysis and Visualizatio</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -879,6 +979,11 @@
       <c r="E21" t="n">
         <v>3</v>
       </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Applied Cyberinfrastruct Conc</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -895,11 +1000,16 @@
         <v>8</v>
       </c>
       <c r="D22" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E22" t="n">
         <v>1</v>
       </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Data Warehousing in the Cloud</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -916,10 +1026,15 @@
         <v>3</v>
       </c>
       <c r="D23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E23" t="n">
         <v>3</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Data Science, Public Interests</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -937,10 +1052,15 @@
         <v>5</v>
       </c>
       <c r="D24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E24" t="n">
         <v>2</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Introduction To Archives</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -961,7 +1081,12 @@
         <v>4</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Artificial Intelligence</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -979,11 +1104,16 @@
         <v>8</v>
       </c>
       <c r="D26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E26" t="n">
         <v>1</v>
       </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Game Development</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1003,7 +1133,12 @@
         <v>4</v>
       </c>
       <c r="E27" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Advanced Game Development</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -1026,6 +1161,11 @@
       <c r="E28" t="n">
         <v>3</v>
       </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Applied NLP</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1042,10 +1182,15 @@
         <v>7</v>
       </c>
       <c r="D29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E29" t="n">
         <v>2</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Neural Networks</t>
+        </is>
       </c>
     </row>
     <row r="30">
@@ -1063,10 +1208,15 @@
         <v>6</v>
       </c>
       <c r="D30" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E30" t="n">
         <v>3</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Social Justice in Info Service</t>
+        </is>
       </c>
     </row>
     <row r="31">
@@ -1089,6 +1239,11 @@
       <c r="E31" t="n">
         <v>3</v>
       </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>STEM Games</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1108,7 +1263,12 @@
         <v>4</v>
       </c>
       <c r="E32" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Leadership &amp; the Info Org</t>
+        </is>
       </c>
     </row>
     <row r="33">
@@ -1126,11 +1286,16 @@
         <v>8</v>
       </c>
       <c r="D33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E33" t="n">
         <v>1</v>
       </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Database Dev And Mgmt</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1147,11 +1312,16 @@
         <v>8</v>
       </c>
       <c r="D34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E34" t="n">
         <v>1</v>
       </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Intro Info Technology</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1168,10 +1338,15 @@
         <v>2</v>
       </c>
       <c r="D35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E35" t="n">
         <v>3</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>User Interf+Website Dsgn</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -1192,7 +1367,12 @@
         <v>4</v>
       </c>
       <c r="E36" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Information Security</t>
+        </is>
       </c>
     </row>
     <row r="37">
@@ -1213,7 +1393,12 @@
         <v>4</v>
       </c>
       <c r="E37" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Science Information</t>
+        </is>
       </c>
     </row>
     <row r="38">
@@ -1231,10 +1416,15 @@
         <v>6</v>
       </c>
       <c r="D38" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E38" t="n">
         <v>3</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>SQL/NoSQL Databases</t>
+        </is>
       </c>
     </row>
     <row r="39">
@@ -1255,7 +1445,12 @@
         <v>4</v>
       </c>
       <c r="E39" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Data for the Semantic Web</t>
+        </is>
       </c>
     </row>
     <row r="40">
@@ -1273,10 +1468,15 @@
         <v>6</v>
       </c>
       <c r="D40" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E40" t="n">
         <v>3</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Intellectual Property/Copyrigh</t>
+        </is>
       </c>
     </row>
     <row r="41">
@@ -1299,6 +1499,11 @@
       <c r="E41" t="n">
         <v>3</v>
       </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Managing the Information Org</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1320,6 +1525,11 @@
       <c r="E42" t="n">
         <v>3</v>
       </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Adv ML Apps</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1339,7 +1549,12 @@
         <v>4</v>
       </c>
       <c r="E43" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Adv Archives: Apprsl &amp; Dscr</t>
+        </is>
       </c>
     </row>
     <row r="44">
@@ -1357,11 +1572,16 @@
         <v>8</v>
       </c>
       <c r="D44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E44" t="n">
         <v>1</v>
       </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Intro Digital Curation/Preserv</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1381,7 +1601,12 @@
         <v>4</v>
       </c>
       <c r="E45" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Intro Applied Technology</t>
+        </is>
       </c>
     </row>
     <row r="46">
@@ -1399,10 +1624,15 @@
         <v>6</v>
       </c>
       <c r="D46" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E46" t="n">
         <v>3</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Managing Digital Info</t>
+        </is>
       </c>
     </row>
     <row r="47">
@@ -1425,6 +1655,11 @@
       <c r="E47" t="n">
         <v>3</v>
       </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Adv Digital Collections</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1441,11 +1676,16 @@
         <v>8</v>
       </c>
       <c r="D48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E48" t="n">
         <v>1</v>
       </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Found Libr+Info Services</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1462,11 +1702,16 @@
         <v>8</v>
       </c>
       <c r="D49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E49" t="n">
         <v>1</v>
       </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Rsrch Mth/Libr+Info Prof</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1483,11 +1728,16 @@
         <v>8</v>
       </c>
       <c r="D50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E50" t="n">
         <v>1</v>
       </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Organization/Information</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1509,6 +1759,11 @@
       <c r="E51" t="n">
         <v>3</v>
       </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Intro to Digital Cultures</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1530,6 +1785,11 @@
       <c r="E52" t="n">
         <v>3</v>
       </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Info Trust and Manipulation</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1546,10 +1806,15 @@
         <v>7</v>
       </c>
       <c r="D53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E53" t="n">
         <v>2</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Ethical Issues in Information</t>
+        </is>
       </c>
     </row>
     <row r="54">
@@ -1570,7 +1835,12 @@
         <v>4</v>
       </c>
       <c r="E54" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Chldrn+Young Adult Lit</t>
+        </is>
       </c>
     </row>
     <row r="55">
@@ -1591,7 +1861,12 @@
         <v>4</v>
       </c>
       <c r="E55" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Early Chlhd+Public Librs</t>
+        </is>
       </c>
     </row>
     <row r="56">
@@ -1609,10 +1884,15 @@
         <v>7</v>
       </c>
       <c r="D56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E56" t="n">
         <v>2</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Cataloging+Metadata Mgmt</t>
+        </is>
       </c>
     </row>
     <row r="57">
@@ -1633,7 +1913,12 @@
         <v>4</v>
       </c>
       <c r="E57" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Info Intermediation</t>
+        </is>
       </c>
     </row>
     <row r="58">
@@ -1651,10 +1936,15 @@
         <v>5</v>
       </c>
       <c r="D58" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E58" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Business Information</t>
+        </is>
       </c>
     </row>
     <row r="59">
@@ -1672,10 +1962,15 @@
         <v>5</v>
       </c>
       <c r="D59" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E59" t="n">
         <v>2</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Introduction To Archives</t>
+        </is>
       </c>
     </row>
     <row r="60">
@@ -1698,6 +1993,11 @@
       <c r="E60" t="n">
         <v>3</v>
       </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Preservation</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1719,6 +2019,11 @@
       <c r="E61" t="n">
         <v>3</v>
       </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Curating &amp; Preserving Media</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1738,7 +2043,12 @@
         <v>4</v>
       </c>
       <c r="E62" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Inf Env/Non-dominant Pers</t>
+        </is>
       </c>
     </row>
     <row r="63">
@@ -1759,7 +2069,12 @@
         <v>4</v>
       </c>
       <c r="E63" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Documnt Divrs Cult+Comms</t>
+        </is>
       </c>
     </row>
     <row r="64">
@@ -1777,11 +2092,16 @@
         <v>8</v>
       </c>
       <c r="D64" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E64" t="n">
         <v>1</v>
       </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Social Justice in Info Service</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1801,7 +2121,12 @@
         <v>4</v>
       </c>
       <c r="E65" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Mktng Library+Info Srvcs</t>
+        </is>
       </c>
     </row>
     <row r="66">
@@ -1819,10 +2144,15 @@
         <v>5</v>
       </c>
       <c r="D66" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E66" t="n">
         <v>2</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Collection Management</t>
+        </is>
       </c>
     </row>
     <row r="67">
@@ -1843,7 +2173,12 @@
         <v>4</v>
       </c>
       <c r="E67" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Rdrs Advisory/Publ Libr</t>
+        </is>
       </c>
     </row>
     <row r="68">
@@ -1864,7 +2199,12 @@
         <v>4</v>
       </c>
       <c r="E68" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Leadership &amp; the Info Org</t>
+        </is>
       </c>
     </row>
     <row r="69">
@@ -1882,11 +2222,16 @@
         <v>8</v>
       </c>
       <c r="D69" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E69" t="n">
         <v>1</v>
       </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Database Dev And Mgmt</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1903,11 +2248,16 @@
         <v>8</v>
       </c>
       <c r="D70" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E70" t="n">
         <v>1</v>
       </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Intro Info Technology</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1927,7 +2277,12 @@
         <v>4</v>
       </c>
       <c r="E71" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Government Information</t>
+        </is>
       </c>
     </row>
     <row r="72">
@@ -1945,10 +2300,15 @@
         <v>2</v>
       </c>
       <c r="D72" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E72" t="n">
         <v>3</v>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>User Interf+Website Dsgn</t>
+        </is>
       </c>
     </row>
     <row r="73">
@@ -1969,7 +2329,12 @@
         <v>4</v>
       </c>
       <c r="E73" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Science Information</t>
+        </is>
       </c>
     </row>
     <row r="74">
@@ -1990,7 +2355,12 @@
         <v>4</v>
       </c>
       <c r="E74" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Data for the Semantic Web</t>
+        </is>
       </c>
     </row>
     <row r="75">
@@ -2008,10 +2378,15 @@
         <v>4</v>
       </c>
       <c r="D75" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E75" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>How to Teach Info Literacy</t>
+        </is>
       </c>
     </row>
     <row r="76">
@@ -2032,7 +2407,12 @@
         <v>4</v>
       </c>
       <c r="E76" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Young Adults+Public Libr</t>
+        </is>
       </c>
     </row>
     <row r="77">
@@ -2053,7 +2433,12 @@
         <v>4</v>
       </c>
       <c r="E77" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>eLearning for Librarians</t>
+        </is>
       </c>
     </row>
     <row r="78">
@@ -2074,7 +2459,12 @@
         <v>4</v>
       </c>
       <c r="E78" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Intellectual Property/Copyrigh</t>
+        </is>
       </c>
     </row>
     <row r="79">
@@ -2097,6 +2487,11 @@
       <c r="E79" t="n">
         <v>3</v>
       </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Learning Design Lib/Info Prof</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2118,6 +2513,11 @@
       <c r="E80" t="n">
         <v>3</v>
       </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Special Topics in LIS</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2139,6 +2539,11 @@
       <c r="E81" t="n">
         <v>3</v>
       </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Managing the Information Org</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2158,7 +2563,12 @@
         <v>4</v>
       </c>
       <c r="E82" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Adv Archives: Apprsl &amp; Dscr</t>
+        </is>
       </c>
     </row>
     <row r="83">
@@ -2181,6 +2591,11 @@
       <c r="E83" t="n">
         <v>3</v>
       </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Comm focused Archives/Museums</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -2197,11 +2612,16 @@
         <v>8</v>
       </c>
       <c r="D84" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E84" t="n">
         <v>1</v>
       </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Intro Digital Curation/Preserv</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -2221,7 +2641,12 @@
         <v>4</v>
       </c>
       <c r="E85" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Intro Applied Technology</t>
+        </is>
       </c>
     </row>
     <row r="86">
@@ -2239,11 +2664,16 @@
         <v>8</v>
       </c>
       <c r="D86" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E86" t="n">
         <v>1</v>
       </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Managing Digital Info</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2265,6 +2695,11 @@
       <c r="E87" t="n">
         <v>3</v>
       </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Adv Digital Collections</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2284,7 +2719,12 @@
         <v>4</v>
       </c>
       <c r="E88" t="n">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Digital Info Mgmt Capstn</t>
+        </is>
       </c>
     </row>
     <row r="89">
@@ -2306,6 +2746,11 @@
       </c>
       <c r="E89" t="n">
         <v>3</v>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Applied Cyberinfrastruct Conc</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>